<commit_message>
fixed a ref link
</commit_message>
<xml_diff>
--- a/data/adult.xlsx
+++ b/data/adult.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msquatrito/Desktop/R/shiny/GlioVis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49337681-A82C-C842-8ED8-32E5C2F70997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E4A030-D4B8-954E-B5C3-1C6C5596C79A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22360" yWindow="2000" windowWidth="27500" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,7 +667,7 @@
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>12</v>

</xml_diff>